<commit_message>
Ejercicios de Haceb Final
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/DataHaceb.xlsx
+++ b/src/main/resources/Data/DataHaceb.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desarrollo\Documents\Clases de Automatización\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desarrollo\CursoAutomatizacion\Ejercicios\PruebaAlkosto\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AAA8A6B-F774-4548-B53F-51E3FD953B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E23F4DE-BD94-406F-93AA-7549A1F2548A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3510" windowWidth="29040" windowHeight="15840" xr2:uid="{96D14C39-5D2A-4532-9077-29507F4797AD}"/>
+    <workbookView xWindow="-19950" yWindow="-435" windowWidth="12960" windowHeight="7965" xr2:uid="{96D14C39-5D2A-4532-9077-29507F4797AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Credenciales" sheetId="1" r:id="rId1"/>
+    <sheet name="Adicionales" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Correo</t>
   </si>
   <si>
-    <t>lmgarzon.lis@hotmail.com</t>
-  </si>
-  <si>
     <t>Nombre</t>
   </si>
   <si>
@@ -63,6 +61,18 @@
   </si>
   <si>
     <t>L1n4L1s85*</t>
+  </si>
+  <si>
+    <t>Cedula</t>
+  </si>
+  <si>
+    <t>FechaNacimiento</t>
+  </si>
+  <si>
+    <t>NumeroTelefono</t>
+  </si>
+  <si>
+    <t>linagl@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -116,10 +126,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -438,7 +448,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -448,34 +458,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -486,4 +496,45 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4591BE42-AF6E-4076-80DB-03924176F6DF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>123456</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7071991</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3123456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>